<commit_message>
update with latest P&L calculation
</commit_message>
<xml_diff>
--- a/gold/excel/crew_summary.xlsx
+++ b/gold/excel/crew_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,30 +451,35 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>flight_hours</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>num_crew</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>?column?</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>flight_hours</t>
+          <t>avg_rate</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>crew_cost_total</t>
+          <t>total_hours_logged</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>crew_cost</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>role_mix</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>crew_flag</t>
         </is>
@@ -483,12 +488,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FL7208</t>
+          <t>FL6679</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT4127</t>
+          <t>RT6565</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -497,35 +502,38 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2.03</v>
       </c>
       <c r="E2" t="n">
-        <v>670</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>6.39</v>
+        <v>140.97</v>
       </c>
       <c r="G2" t="n">
-        <v>4281.3</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I2" t="b">
+        <v>28</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3947.22</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FL2825</t>
+          <t>FL1976</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT2741</t>
+          <t>RT5358</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -534,35 +542,38 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>3.68</v>
       </c>
       <c r="E3" t="n">
-        <v>661.4</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>3.52</v>
+        <v>172.18</v>
       </c>
       <c r="G3" t="n">
-        <v>2328.13</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="H3" t="n">
+        <v>7231.59</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FL9519</t>
+          <t>FL4876</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RT0983</t>
+          <t>RT4447</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -571,35 +582,38 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>4.95</v>
       </c>
       <c r="E4" t="n">
-        <v>656.6</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
-        <v>6.1</v>
+        <v>182.63</v>
       </c>
       <c r="G4" t="n">
-        <v>4005.26</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I4" t="b">
+        <v>49</v>
+      </c>
+      <c r="H4" t="n">
+        <v>8948.68</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FL4177</t>
+          <t>FL1198</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RT0983</t>
+          <t>RT6565</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -608,183 +622,198 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2.03</v>
       </c>
       <c r="E5" t="n">
-        <v>650.1</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>2.48</v>
+        <v>140.69</v>
       </c>
       <c r="G5" t="n">
-        <v>1612.25</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I5" t="b">
+        <v>28</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3939.37</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FL6596</t>
+          <t>FL3066</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RT8820</t>
+          <t>RT6474</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>wide-body</t>
+          <t>narrow-body</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E6" t="n">
-        <v>642.6</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
-        <v>7.7</v>
+        <v>141.86</v>
       </c>
       <c r="G6" t="n">
-        <v>4948.02</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I6" t="b">
+        <v>28</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3972.01</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FL4773</t>
+          <t>FL5388</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RT0983</t>
+          <t>RT5358</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>wide-body</t>
+          <t>narrow-body</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>3.68</v>
       </c>
       <c r="E7" t="n">
-        <v>653.7</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
-        <v>4.44</v>
+        <v>178.95</v>
       </c>
       <c r="G7" t="n">
-        <v>2902.43</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I7" t="b">
+        <v>42</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7516.03</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FL9323</t>
+          <t>FL5301</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RT0983</t>
+          <t>RT6474</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>wide-body</t>
+          <t>narrow-body</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E8" t="n">
-        <v>672.3</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>1.21</v>
+        <v>146.74</v>
       </c>
       <c r="G8" t="n">
-        <v>813.48</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4108.63</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FL1288</t>
+          <t>FL7875</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RT4127</t>
+          <t>RT4447</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>regional jet</t>
+          <t>narrow-body</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>4.95</v>
       </c>
       <c r="E9" t="n">
-        <v>644</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
-        <v>3.17</v>
+        <v>186.75</v>
       </c>
       <c r="G9" t="n">
-        <v>2041.48</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I9" t="b">
+        <v>49</v>
+      </c>
+      <c r="H9" t="n">
+        <v>9150.629999999999</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FL8734</t>
+          <t>FL6369</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RT0983</t>
+          <t>RT5358</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -793,35 +822,38 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>3.68</v>
       </c>
       <c r="E10" t="n">
-        <v>655.8</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>3.04</v>
+        <v>181.68</v>
       </c>
       <c r="G10" t="n">
-        <v>1993.63</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="H10" t="n">
+        <v>7630.55</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FL3561</t>
+          <t>FL7466</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RT2741</t>
+          <t>RT5358</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -830,24 +862,627 @@
         </is>
       </c>
       <c r="D11" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>181.52</v>
+      </c>
+      <c r="G11" t="n">
+        <v>42</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7623.73</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FL3108</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>RT6474</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>7</v>
+      </c>
+      <c r="F12" t="n">
+        <v>151.26</v>
+      </c>
+      <c r="G12" t="n">
+        <v>28</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4235.35</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>FL4736</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RT7502</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="n">
+        <v>145.26</v>
+      </c>
+      <c r="G13" t="n">
+        <v>21</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3050.44</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J13" t="b">
         <v>1</v>
       </c>
-      <c r="E11" t="n">
-        <v>668.9</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2.97</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1986.63</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2P / 2A</t>
-        </is>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>FL5961</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>RT6259</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>wide-body</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>7.25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" t="n">
+        <v>195.95</v>
+      </c>
+      <c r="G14" t="n">
+        <v>90</v>
+      </c>
+      <c r="H14" t="n">
+        <v>17635.14</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2P / 8A</t>
+        </is>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>FL2734</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>RT6259</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>wide-body</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>7.25</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" t="n">
+        <v>195.18</v>
+      </c>
+      <c r="G15" t="n">
+        <v>90</v>
+      </c>
+      <c r="H15" t="n">
+        <v>17566.2</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2P / 8A</t>
+        </is>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FL1013</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>RT6259</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>wide-body</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>7.25</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
+        <v>197.14</v>
+      </c>
+      <c r="G16" t="n">
+        <v>90</v>
+      </c>
+      <c r="H16" t="n">
+        <v>17742.42</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2P / 8A</t>
+        </is>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>FL5705</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>RT6565</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="n">
+        <v>136.83</v>
+      </c>
+      <c r="G17" t="n">
+        <v>32</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4378.61</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2P / 6A</t>
+        </is>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FL1524</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>RT5358</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" t="n">
+        <v>168.54</v>
+      </c>
+      <c r="G18" t="n">
+        <v>48</v>
+      </c>
+      <c r="H18" t="n">
+        <v>8089.73</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2P / 6A</t>
+        </is>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>FL5421</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>RT4447</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="n">
+        <v>170.64</v>
+      </c>
+      <c r="G19" t="n">
+        <v>56</v>
+      </c>
+      <c r="H19" t="n">
+        <v>9555.610000000001</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2P / 6A</t>
+        </is>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>FL6133</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>RT4447</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8</v>
+      </c>
+      <c r="F20" t="n">
+        <v>173.32</v>
+      </c>
+      <c r="G20" t="n">
+        <v>56</v>
+      </c>
+      <c r="H20" t="n">
+        <v>9705.93</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2P / 6A</t>
+        </is>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>FL8299</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>RT7502</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>regional jet</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E21" t="n">
+        <v>5</v>
+      </c>
+      <c r="F21" t="n">
+        <v>163.16</v>
+      </c>
+      <c r="G21" t="n">
+        <v>15</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2447.45</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2P / 3A</t>
+        </is>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FL5785</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>RT7502</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E22" t="n">
+        <v>7</v>
+      </c>
+      <c r="F22" t="n">
+        <v>144.61</v>
+      </c>
+      <c r="G22" t="n">
+        <v>21</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3036.82</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FL5235</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>RT4447</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="E23" t="n">
+        <v>7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>179.91</v>
+      </c>
+      <c r="G23" t="n">
+        <v>49</v>
+      </c>
+      <c r="H23" t="n">
+        <v>8815.530000000001</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>FL5689</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>RT6565</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="E24" t="n">
+        <v>7</v>
+      </c>
+      <c r="F24" t="n">
+        <v>145.35</v>
+      </c>
+      <c r="G24" t="n">
+        <v>28</v>
+      </c>
+      <c r="H24" t="n">
+        <v>4069.73</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>FL8121</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>RT7502</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>narrow-body</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E25" t="n">
+        <v>7</v>
+      </c>
+      <c r="F25" t="n">
+        <v>147.4</v>
+      </c>
+      <c r="G25" t="n">
+        <v>21</v>
+      </c>
+      <c r="H25" t="n">
+        <v>3095.32</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2P / 5A</t>
+        </is>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>FL1990</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>RT6259</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>wide-body</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>7.25</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10</v>
+      </c>
+      <c r="F26" t="n">
+        <v>198.07</v>
+      </c>
+      <c r="G26" t="n">
+        <v>90</v>
+      </c>
+      <c r="H26" t="n">
+        <v>17826.48</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2P / 8A</t>
+        </is>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>